<commit_message>
Se adiciona clase para paginar tabla con angularjs
</commit_message>
<xml_diff>
--- a/Resources/base-mide.xlsx
+++ b/Resources/base-mide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\serviceMide\testing\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\serviceMide\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
   <si>
     <t>PRODUCTO MIDE</t>
   </si>
@@ -201,9 +201,6 @@
     <t>SI</t>
   </si>
   <si>
-    <t>UNIVERSIDAD DE LOS ANDES</t>
-  </si>
-  <si>
     <t>UNIVERSIDAD NACIONAL DE COLOMBIA</t>
   </si>
   <si>
@@ -217,6 +214,60 @@
   </si>
   <si>
     <t>UNIVERSIDADES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIVERSIDAD DE LOS ANDES </t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD GRAN COLOMBIANA</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD PARA TODOS</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DE TUNJA</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DEL IBAGE</t>
+  </si>
+  <si>
+    <t>PONTIFICIA UNIVERSIDAD DEL VALLE</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DE LOS FLORES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DE CALI</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DE MEDELLIN</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DEL NORTE DEL VALLE</t>
+  </si>
+  <si>
+    <t>PONTIFICIA UNIVERSIDAD PACIFICO</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DEL PACIFICO NORTE</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD PLAN NACIONAL</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DE LAS MARIAS</t>
+  </si>
+  <si>
+    <t>UNIVERSIDAD DEL PACICO</t>
+  </si>
+  <si>
+    <t>PONTIFICIA UNIVERSIDAD DE LA REGION</t>
+  </si>
+  <si>
+    <t>INSTITUCION UNIVERSITARIA</t>
   </si>
 </sst>
 </file>
@@ -610,15 +661,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -652,13 +703,13 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12385</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="2">
-        <v>12345</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -675,13 +726,13 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>123456</v>
+        <v>12386</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -698,13 +749,13 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>234567</v>
+        <v>12387</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -721,13 +772,13 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>345678</v>
+        <v>12388</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -744,13 +795,13 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2">
-        <v>456789</v>
+        <v>12389</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -763,6 +814,351 @@
       </c>
       <c r="G6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12390</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12391</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>12392</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12393</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12394</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12395</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12396</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12397</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2">
+        <v>12398</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2">
+        <v>12399</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2">
+        <v>12400</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2">
+        <v>12401</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2">
+        <v>12402</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2">
+        <v>12403</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2">
+        <v>12404</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>